<commit_message>
Be vs NL AH
</commit_message>
<xml_diff>
--- a/Web Scraping/Berrie.xlsx
+++ b/Web Scraping/Berrie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="AH" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AH" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G660"/>
+  <dimension ref="A1:G754"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23382,6 +23382,3484 @@
         </is>
       </c>
       <c r="G660" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>Noten-, boter- of zandkoekjes</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E661" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F661" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G661" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>Krokante muesli 4 noten</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>3.29</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E662" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F662" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G662" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>gezouten notenmix 150g</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E663" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F663" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G663" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>Paranoten</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E664" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F664" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G664" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>Bakkerskruidnoten</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Price not found</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E665" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F665" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G665" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>Borrelnootjes</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Price not found</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E666" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F666" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G666" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>Zaden &amp; pitten</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E667" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F667" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G667" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E668" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F668" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G668" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E669" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F669" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G669" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E670" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F670" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G670" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>Zoute sticks</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E671" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F671" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G671" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>Roomboter kaaszoutjes</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E672" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F672" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G672" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>Japanse mix</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E673" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F673" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G673" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>Roomboter kaaskoekjes</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E674" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F674" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G674" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>Roomboter kaaskoekjes</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E675" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F675" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G675" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>Pitten</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E676" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F676" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G676" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>Zaden &amp; pitten</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E677" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F677" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G677" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>Pijnboompitten</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>2.49</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E678" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F678" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G678" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>Borrelnootjes</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Price not found</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E679" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F679" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G679" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E680" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F680" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G680" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>Cashewnoten &amp; pinda's</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>3.49</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E681" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F681" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G681" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E682" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F682" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G682" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E683" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F683" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G683" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>5.28</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E685" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F685" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G685" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>Amandelen</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E686" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G686" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>Amandelen</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E687" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F687" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G687" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>Ongebrande amandelen</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>1.98</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E688" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F688" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G688" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>Cashewnoten &amp; pinda's</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>3.49</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E690" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F690" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G690" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>Pinda-maïsmix</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E691" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>Pinda's</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E692" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F692" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G692" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>Dry roasted pinda's</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E693" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F693" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G693" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>Dry roasted pinda's</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E694" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F694" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G694" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>Dry roasted notenmix</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>Koekhappers rozijnen</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>Mini-roomboterrozijnenbollen</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E697" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F697" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G697" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>Koekhappers minder suiker of rozijn</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F698" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G698" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>Chocoladerozijnen</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F699" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G699" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>Cranberry's of cranberry's &amp; rozijnen melange</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E700" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F700" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G700" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>Macadamia's</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F701" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G701" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>Macadamiamix</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>2.89</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F702" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G702" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>Macadamiamix</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E703" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F703" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G703" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>Candy bars</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F704" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G704" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F705" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G705" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>Chocolade pindakoeken</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>Pindarotsjes</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>Noten-, boter- of zandkoekjes</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F708" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>Krokante muesli 4 noten</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>3.29</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>900 g</t>
+        </is>
+      </c>
+      <c r="E709" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F709" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G709" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>gezouten notenmix 150g</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>150 g</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F710" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G710" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>Paranoten</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F711" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G711" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>Bakkerskruidnoten</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Price not found</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E712" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F712" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G712" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>Borrelnootjes</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Price not found</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F713" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G713" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>Zaden &amp; pitten</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>120 g</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F714" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G714" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E715" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F715" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G715" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F717" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G717" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>Zoute sticks</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E718" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F718" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G718" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>Roomboter kaaszoutjes</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>100 g</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F719" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G719" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>Japanse mix</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F720" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G720" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>Roomboter kaaskoekjes</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>100 g</t>
+        </is>
+      </c>
+      <c r="E721" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F721" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G721" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>Roomboter kaaskoekjes</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>100 g</t>
+        </is>
+      </c>
+      <c r="E722" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F722" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G722" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>Pitten</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E723" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F723" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G723" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>Zaden &amp; pitten</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>120 g</t>
+        </is>
+      </c>
+      <c r="E724" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F724" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G724" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>Pijnboompitten</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>2.49</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>50 g</t>
+        </is>
+      </c>
+      <c r="E725" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F725" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G725" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>Borrelnootjes</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Price not found</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>Weight not found</t>
+        </is>
+      </c>
+      <c r="E726" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E727" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F727" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G727" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>Cashewnoten &amp; pinda's</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>3.49</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E728" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F728" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G728" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E729" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F729" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G729" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E730" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F730" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G730" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>5.28</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>500 g.</t>
+        </is>
+      </c>
+      <c r="E731" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F731" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G731" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>Cashewnoten</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E732" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F732" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G732" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>Amandelen</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E733" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F733" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G733" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>Amandelen</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>200 g.</t>
+        </is>
+      </c>
+      <c r="E734" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F734" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G734" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>Ongebrande amandelen</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>1.98</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E735" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F735" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G735" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>Cashewnoten &amp; pinda's</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>3.49</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E736" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F736" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G736" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E737" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F737" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G737" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>Pinda-maïsmix</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>150 g</t>
+        </is>
+      </c>
+      <c r="E738" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F738" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G738" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>Pinda's</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E739" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F739" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G739" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>Dry roasted pinda's</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>225 g</t>
+        </is>
+      </c>
+      <c r="E740" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F740" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G740" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>Dry roasted pinda's</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>225 g</t>
+        </is>
+      </c>
+      <c r="E741" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F741" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G741" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>Dry roasted notenmix</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>125 g</t>
+        </is>
+      </c>
+      <c r="E742" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F742" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G742" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>Koekhappers rozijnen</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D743" t="inlineStr">
+        <is>
+          <t>6+1 gratis</t>
+        </is>
+      </c>
+      <c r="E743" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F743" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G743" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>Mini-roomboterrozijnenbollen</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>9 stuks</t>
+        </is>
+      </c>
+      <c r="E744" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F744" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G744" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>Koekhappers minder suiker of rozijn</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>6 stuks.</t>
+        </is>
+      </c>
+      <c r="E745" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F745" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G745" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>Chocoladerozijnen</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E746" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F746" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G746" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>Cranberry's of cranberry's &amp; rozijnen melange</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E747" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F747" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G747" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>Macadamia's</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>125 g</t>
+        </is>
+      </c>
+      <c r="E748" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F748" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G748" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>Macadamiamix</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>2.89</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>130 g</t>
+        </is>
+      </c>
+      <c r="E749" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F749" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G749" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>Macadamiamix</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>2.59</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>130 g</t>
+        </is>
+      </c>
+      <c r="E750" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F750" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G750" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>Candy bars</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>6x50 g</t>
+        </is>
+      </c>
+      <c r="E751" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F751" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G751" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>Melkchocolade pinda's</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>200 g</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F752" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G752" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>Chocolade pindakoeken</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>Inhoud: 6 stuks, 200 g</t>
+        </is>
+      </c>
+      <c r="E753" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F753" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G753" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>Pindarotsjes</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>No promo price</t>
+        </is>
+      </c>
+      <c r="D754" t="inlineStr">
+        <is>
+          <t>250 g</t>
+        </is>
+      </c>
+      <c r="E754" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F754" t="inlineStr">
+        <is>
+          <t>Aldi</t>
+        </is>
+      </c>
+      <c r="G754" t="inlineStr">
         <is>
           <t>2025-06-02</t>
         </is>

</xml_diff>